<commit_message>
feat agregar step envio conciliacion por email
</commit_message>
<xml_diff>
--- a/src/main/resources/reconciliation_report.xlsx
+++ b/src/main/resources/reconciliation_report.xlsx
@@ -664,10 +664,10 @@
     <t>058405267</t>
   </si>
   <si>
-    <t>TRANSACCIÓN DUPLICADA JPAT 1</t>
-  </si>
-  <si>
-    <t>TRANSACCIÓN DUPLICADA JPAT 2</t>
+    <t>TRANSACCION DUPLICADA JPAT 1</t>
+  </si>
+  <si>
+    <t>TRANSACCION DUPLICADA JPAT 2</t>
   </si>
   <si>
     <t>51827790250004</t>

</xml_diff>